<commit_message>
tambah export di kelompok
</commit_message>
<xml_diff>
--- a/public/templates/template_desa.xlsx
+++ b/public/templates/template_desa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Testing\AbsenCAI\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E484345-0C45-4E6C-BE2F-108D44E5D3E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EB2E6E1-C7F4-4448-BF67-2028509A3B15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,9 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>DESA</t>
-  </si>
-  <si>
     <t>BATAM</t>
   </si>
   <si>
@@ -37,6 +34,9 @@
   </si>
   <si>
     <t>RINGROAD</t>
+  </si>
+  <si>
+    <t>desa</t>
   </si>
 </sst>
 </file>
@@ -356,30 +356,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:A7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>